<commit_message>
Kvalitet samt opfølgning ajourført
</commit_message>
<xml_diff>
--- a/reports/r4/opf�lgning.xlsx
+++ b/reports/r4/opf�lgning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="9270" windowHeight="4665" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9270" windowHeight="4665"/>
   </bookViews>
   <sheets>
     <sheet name="Opfølgning" sheetId="1" r:id="rId1"/>
@@ -518,12 +518,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -533,6 +527,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -965,7 +965,7 @@
       <c r="I4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="35" t="s">
+      <c r="J4" s="33" t="s">
         <v>74</v>
       </c>
       <c r="K4" s="25" t="s">
@@ -979,11 +979,11 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
@@ -1013,27 +1013,27 @@
         <v>60</v>
       </c>
       <c r="H6" s="18">
-        <f>$M1-H1</f>
+        <f t="shared" ref="H6:M6" si="0">$M1-H1</f>
         <v>51</v>
       </c>
       <c r="I6" s="18">
-        <f>$M1-I1</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="J6" s="11">
-        <f>$M1-J1</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="K6" s="11">
-        <f>$M1-K1</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L6" s="20">
-        <f>$M1-L1</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="M6" s="18">
-        <f>$M1-M1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1064,27 +1064,27 @@
         <v>82</v>
       </c>
       <c r="H7" s="19">
-        <f>$B6-H6</f>
+        <f t="shared" ref="H7:M7" si="1">$B6-H6</f>
         <v>91</v>
       </c>
       <c r="I7" s="19">
-        <f>$B6-I6</f>
+        <f t="shared" si="1"/>
         <v>117</v>
       </c>
       <c r="J7" s="12">
-        <f>$B6-J6</f>
+        <f t="shared" si="1"/>
         <v>128</v>
       </c>
       <c r="K7" s="12">
-        <f>$B6-K6</f>
+        <f t="shared" si="1"/>
         <v>135</v>
       </c>
       <c r="L7" s="21">
-        <f>$B6-L6</f>
+        <f t="shared" si="1"/>
         <v>139</v>
       </c>
       <c r="M7" s="19">
-        <f>$B6-M6</f>
+        <f t="shared" si="1"/>
         <v>142</v>
       </c>
     </row>
@@ -1210,44 +1210,47 @@
         <v>0</v>
       </c>
       <c r="C13" s="18">
-        <v>0</v>
+        <f t="shared" ref="C13:F13" si="2">ROUND(($C$16-C16+75)/$C$16,2)*100</f>
+        <v>9</v>
       </c>
       <c r="D13" s="18">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
       <c r="E13" s="18">
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>30</v>
       </c>
       <c r="F13" s="18">
-        <f t="shared" ref="F13:H13" si="0">ROUND(($E$16-F16+47)/$E$16,2)*100</f>
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>42</v>
       </c>
       <c r="G13" s="18">
-        <f t="shared" si="0"/>
-        <v>23</v>
+        <f>ROUND(($C$16-G16+75)/$C$16,2)*100</f>
+        <v>42</v>
       </c>
       <c r="H13" s="18">
-        <f t="shared" si="0"/>
-        <v>33</v>
+        <f t="shared" ref="H13:I13" si="3">ROUND(($C$16-H16+75)/$C$16,2)*100</f>
+        <v>50</v>
       </c>
       <c r="I13" s="18">
-        <f>ROUND(($E$16-I16+47)/$E$16,2)*100</f>
-        <v>33</v>
+        <f t="shared" si="3"/>
+        <v>50</v>
       </c>
       <c r="J13" s="11">
-        <f>ROUND(($E$16-J16+47)/$E$16,2)*100</f>
-        <v>57.999999999999993</v>
+        <f>ROUND(($C$16-J16+75)/$C$16,2)*100</f>
+        <v>70</v>
       </c>
       <c r="K13" s="11">
-        <f>ROUND(($E$16-K16+47)/$E$16,2)*100</f>
-        <v>84</v>
-      </c>
-      <c r="L13" s="20">
-        <f>ROUND(($E$16-L16+47)/$E$16,2)*100</f>
-        <v>94</v>
+        <f t="shared" ref="K13:L13" si="4">ROUND(($C$16-K16+75)/$C$16,2)*100</f>
+        <v>90</v>
+      </c>
+      <c r="L13" s="11">
+        <f t="shared" si="4"/>
+        <v>99</v>
       </c>
       <c r="M13" s="18">
-        <f t="shared" ref="G13:M13" si="1">ROUND(($E$16-M16)/$E$16,2)*100</f>
+        <f t="shared" ref="M13" si="5">ROUND(($E$16-M16)/$E$16,2)*100</f>
         <v>100</v>
       </c>
     </row>
@@ -1259,8 +1262,12 @@
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
+      <c r="F14" s="18">
+        <v>48</v>
+      </c>
+      <c r="G14" s="18">
+        <v>48</v>
+      </c>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
       <c r="J14" s="11"/>
@@ -1297,15 +1304,15 @@
         <f>B16-228</f>
         <v>672</v>
       </c>
-      <c r="E16" s="31">
+      <c r="E16" s="29">
         <f>B16-260</f>
         <v>640</v>
       </c>
-      <c r="F16" s="31">
+      <c r="F16" s="29">
         <f>B16-358</f>
         <v>542</v>
       </c>
-      <c r="G16" s="31">
+      <c r="G16" s="29">
         <f>B16-358</f>
         <v>542</v>
       </c>
@@ -1349,15 +1356,15 @@
         <v>596.70000000000005</v>
       </c>
       <c r="E17" s="18">
-        <f t="shared" ref="E17:G17" si="2">$B$17*(100-E11)/100</f>
+        <f t="shared" ref="E17:G17" si="6">$B$17*(100-E11)/100</f>
         <v>520.20000000000005</v>
       </c>
       <c r="F17" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>359.55</v>
       </c>
       <c r="G17" s="18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>344.25</v>
       </c>
       <c r="H17" s="18"/>
@@ -1409,11 +1416,11 @@
     </row>
     <row r="23" spans="1:13" ht="27.75" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="28"/>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
       <c r="G23" s="27"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
@@ -1443,66 +1450,66 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="3" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3" style="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3" style="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3" style="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3" style="28" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3" style="30" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" style="28" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3" style="30" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3" style="28" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29" t="s">
+      <c r="E1" s="36"/>
+      <c r="F1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29" t="s">
+      <c r="I1" s="36"/>
+      <c r="J1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="K1" s="29"/>
+      <c r="K1" s="36"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="28" t="s">
         <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="28" t="s">
         <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="28" t="s">
         <v>42</v>
       </c>
       <c r="G2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" s="30" t="s">
+      <c r="H2" s="28" t="s">
         <v>42</v>
       </c>
       <c r="I2" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="30" t="s">
+      <c r="J2" s="28" t="s">
         <v>42</v>
       </c>
       <c r="K2" t="s">
@@ -1523,16 +1530,16 @@
       <c r="A5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="30">
+      <c r="B5" s="28">
         <v>3</v>
       </c>
-      <c r="F5" s="30">
+      <c r="F5" s="28">
         <v>3</v>
       </c>
-      <c r="H5" s="30">
+      <c r="H5" s="28">
         <v>2</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="28">
         <v>3</v>
       </c>
       <c r="K5">
@@ -1543,22 +1550,22 @@
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="30">
-        <v>4</v>
-      </c>
-      <c r="D6" s="30">
-        <v>4</v>
-      </c>
-      <c r="F6" s="30">
+      <c r="B6" s="28">
+        <v>4</v>
+      </c>
+      <c r="D6" s="28">
+        <v>4</v>
+      </c>
+      <c r="F6" s="28">
         <v>4</v>
       </c>
       <c r="G6">
         <v>3</v>
       </c>
-      <c r="H6" s="30">
-        <v>4</v>
-      </c>
-      <c r="J6" s="30">
+      <c r="H6" s="28">
+        <v>4</v>
+      </c>
+      <c r="J6" s="28">
         <v>4</v>
       </c>
       <c r="K6">
@@ -1569,25 +1576,25 @@
       <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="30">
-        <v>4</v>
-      </c>
-      <c r="D7" s="30">
+      <c r="B7" s="28">
+        <v>4</v>
+      </c>
+      <c r="D7" s="28">
         <v>4</v>
       </c>
       <c r="E7">
         <v>4</v>
       </c>
-      <c r="F7" s="30">
+      <c r="F7" s="28">
         <v>4</v>
       </c>
       <c r="G7">
         <v>7</v>
       </c>
-      <c r="H7" s="30">
-        <v>4</v>
-      </c>
-      <c r="J7" s="30">
+      <c r="H7" s="28">
+        <v>4</v>
+      </c>
+      <c r="J7" s="28">
         <v>4</v>
       </c>
       <c r="K7">
@@ -1598,28 +1605,28 @@
       <c r="A8" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="28">
         <v>2.5</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="28">
         <v>2.5</v>
       </c>
-      <c r="F8" s="30">
+      <c r="F8" s="28">
         <v>2.5</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
-      <c r="H8" s="30">
+      <c r="H8" s="28">
         <v>2.5</v>
       </c>
       <c r="I8">
         <v>4</v>
       </c>
-      <c r="J8" s="30">
+      <c r="J8" s="28">
         <v>2.5</v>
       </c>
       <c r="K8">
@@ -1630,22 +1637,22 @@
       <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="30">
+      <c r="B9" s="28">
         <v>2.5</v>
       </c>
       <c r="E9">
         <v>6</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="28">
         <v>2.5</v>
       </c>
       <c r="G9">
         <v>9</v>
       </c>
-      <c r="H9" s="30">
+      <c r="H9" s="28">
         <v>2.5</v>
       </c>
-      <c r="J9" s="30">
+      <c r="J9" s="28">
         <v>3</v>
       </c>
       <c r="K9">
@@ -1656,25 +1663,25 @@
       <c r="A10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="28">
         <v>4</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
-      <c r="D10" s="30">
+      <c r="D10" s="28">
         <v>4</v>
       </c>
       <c r="E10" s="22">
         <v>6</v>
       </c>
-      <c r="F10" s="30">
+      <c r="F10" s="28">
         <v>4</v>
       </c>
       <c r="G10" s="22">
         <v>5</v>
       </c>
-      <c r="H10" s="30">
+      <c r="H10" s="28">
         <v>4</v>
       </c>
       <c r="I10">
@@ -1688,22 +1695,22 @@
       <c r="A11" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="30">
-        <v>4</v>
-      </c>
-      <c r="D11" s="30">
-        <v>4</v>
-      </c>
-      <c r="F11" s="30">
-        <v>4</v>
-      </c>
-      <c r="H11" s="30">
+      <c r="B11" s="28">
+        <v>4</v>
+      </c>
+      <c r="D11" s="28">
+        <v>4</v>
+      </c>
+      <c r="F11" s="28">
+        <v>4</v>
+      </c>
+      <c r="H11" s="28">
         <v>4</v>
       </c>
       <c r="I11" s="22">
         <v>2</v>
       </c>
-      <c r="J11" s="30">
+      <c r="J11" s="28">
         <v>4</v>
       </c>
       <c r="K11" s="22">
@@ -1714,22 +1721,22 @@
       <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="30">
-        <v>4</v>
-      </c>
-      <c r="D12" s="30">
-        <v>4</v>
-      </c>
-      <c r="F12" s="30">
+      <c r="B12" s="28">
+        <v>4</v>
+      </c>
+      <c r="D12" s="28">
+        <v>4</v>
+      </c>
+      <c r="F12" s="28">
         <v>4</v>
       </c>
       <c r="G12">
         <v>4</v>
       </c>
-      <c r="H12" s="30">
-        <v>4</v>
-      </c>
-      <c r="J12" s="30">
+      <c r="H12" s="28">
+        <v>4</v>
+      </c>
+      <c r="J12" s="28">
         <v>4</v>
       </c>
       <c r="K12" s="22">
@@ -1740,16 +1747,16 @@
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="30">
-        <v>4</v>
-      </c>
-      <c r="F13" s="30">
-        <v>4</v>
-      </c>
-      <c r="H13" s="30">
-        <v>4</v>
-      </c>
-      <c r="J13" s="30">
+      <c r="D13" s="28">
+        <v>4</v>
+      </c>
+      <c r="F13" s="28">
+        <v>4</v>
+      </c>
+      <c r="H13" s="28">
+        <v>4</v>
+      </c>
+      <c r="J13" s="28">
         <v>4</v>
       </c>
       <c r="K13" s="22">
@@ -1760,19 +1767,19 @@
       <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="30">
+      <c r="D14" s="28">
         <v>2</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
-      <c r="F14" s="30">
+      <c r="F14" s="28">
         <v>2</v>
       </c>
-      <c r="H14" s="30">
+      <c r="H14" s="28">
         <v>2</v>
       </c>
-      <c r="J14" s="30">
+      <c r="J14" s="28">
         <v>2</v>
       </c>
       <c r="K14" s="22">
@@ -1783,16 +1790,16 @@
       <c r="A15" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="30">
+      <c r="D15" s="28">
         <v>8</v>
       </c>
-      <c r="F15" s="30">
+      <c r="F15" s="28">
         <v>7</v>
       </c>
-      <c r="H15" s="30">
+      <c r="H15" s="28">
         <v>8</v>
       </c>
-      <c r="J15" s="30">
+      <c r="J15" s="28">
         <v>8</v>
       </c>
       <c r="L15" t="s">
@@ -1822,14 +1829,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="33">
+      <c r="A1" s="31">
         <f>B2*D2+B26*D26</f>
         <v>0.5573611111111112</v>
       </c>
@@ -1838,24 +1845,24 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="33">
+      <c r="B2" s="31">
         <f>C3*E3+C16*E16+C22*E22</f>
         <v>0.91472222222222244</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="33"/>
-      <c r="C3" s="34">
+      <c r="B3" s="31"/>
+      <c r="C3" s="32">
         <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
         <v>0.91250000000000009</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="32" t="s">
         <v>53</v>
       </c>
       <c r="E3">
@@ -1864,143 +1871,143 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="D4" s="34">
+      <c r="D4" s="32">
         <f>E5*G5</f>
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="E5" s="34">
+      <c r="E5" s="32">
         <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="D6" s="34">
+      <c r="D6" s="32">
         <f>E7*G7+E8*G8</f>
         <v>0.85000000000000009</v>
       </c>
       <c r="E6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>0.9</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>0.8</v>
       </c>
       <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="D9" s="34">
+      <c r="D9" s="32">
         <f>E10*G10+E11*G11+E12*G12</f>
         <v>0.85</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="E10" s="34">
+      <c r="E10" s="32">
         <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="E11" s="34">
+      <c r="E11" s="32">
         <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="E12" s="34">
+      <c r="E12" s="32">
         <v>0.7</v>
       </c>
       <c r="F12" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="D13" s="34">
+      <c r="D13" s="32">
         <f>E14*G14+E15*G15</f>
         <v>0.95</v>
       </c>
       <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="34">
+      <c r="E14" s="32">
         <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="34">
+      <c r="E15" s="32">
         <v>0.9</v>
       </c>
       <c r="F15" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="C16" s="34">
+      <c r="C16" s="32">
         <f>D17*F17+D18*F18+D21*F21</f>
         <v>0.96500000000000008</v>
       </c>
@@ -2013,58 +2020,58 @@
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="D17" s="34">
+      <c r="D17" s="32">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="34">
+      <c r="F17" s="32">
         <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="1:7">
-      <c r="D18" s="34">
+      <c r="D18" s="32">
         <f>E19*G19+E20*G20</f>
         <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="34">
+      <c r="F18" s="32">
         <v>0.45</v>
       </c>
     </row>
     <row r="19" spans="1:7">
-      <c r="E19" s="34">
+      <c r="E19" s="32">
         <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:7">
-      <c r="E20" s="34">
+      <c r="E20" s="32">
         <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:7">
-      <c r="D21" s="34">
+      <c r="D21" s="32">
         <v>0.7</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="32">
         <v>0.45</v>
       </c>
     </row>
@@ -2082,7 +2089,7 @@
       </c>
     </row>
     <row r="23" spans="1:7">
-      <c r="D23" s="34">
+      <c r="D23" s="32">
         <v>1</v>
       </c>
       <c r="E23" t="s">
@@ -2094,7 +2101,7 @@
       </c>
     </row>
     <row r="24" spans="1:7">
-      <c r="D24" s="34">
+      <c r="D24" s="32">
         <v>1</v>
       </c>
       <c r="E24" t="s">
@@ -2106,7 +2113,7 @@
       </c>
     </row>
     <row r="25" spans="1:7">
-      <c r="D25" s="34">
+      <c r="D25" s="32">
         <v>0.6</v>
       </c>
       <c r="E25" t="s">
@@ -2118,37 +2125,37 @@
       </c>
     </row>
     <row r="26" spans="1:7">
-      <c r="B26" s="34">
+      <c r="B26" s="32">
         <f>C27*E27</f>
         <v>0.2</v>
       </c>
       <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="1:7">
-      <c r="C27" s="34">
+      <c r="C27" s="32">
         <f>D28*F28</f>
         <v>0.2</v>
       </c>
       <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="D28" s="34">
+      <c r="D28" s="32">
         <v>0.2</v>
       </c>
       <c r="E28" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="34">
+      <c r="F28" s="32">
         <v>1</v>
       </c>
     </row>
@@ -2164,35 +2171,35 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C32" s="34">
-        <v>1</v>
-      </c>
-      <c r="D32" s="34">
+      <c r="C32" s="32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="32">
         <f>D34*$C$34+D39*$C$39</f>
         <v>0.41874999999999996</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="32">
         <f>E34*$C$34+E39*$C$39</f>
         <v>0.48229166666666667</v>
       </c>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="36"/>
+      <c r="A33" s="34"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="34">
+      <c r="C34" s="32">
         <v>0.25</v>
       </c>
-      <c r="D34" s="34">
-        <v>1</v>
-      </c>
-      <c r="E34" s="34">
+      <c r="D34" s="32">
+        <v>1</v>
+      </c>
+      <c r="E34" s="32">
         <v>1</v>
       </c>
     </row>
@@ -2212,50 +2219,50 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="C39" s="34">
+      <c r="C39" s="32">
         <v>0.75</v>
       </c>
-      <c r="D39" s="34">
+      <c r="D39" s="32">
         <f>D40*$C$40+D58*$C$58</f>
         <v>0.22499999999999998</v>
       </c>
-      <c r="E39" s="34">
+      <c r="E39" s="32">
         <f>E40*$C$40+E58*$C$58</f>
         <v>0.30972222222222223</v>
       </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="D40" s="34">
+      <c r="C40" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="D40" s="32">
         <f>D41*$C$41+D45*$C$45+D53*$C$53</f>
         <v>0.44999999999999996</v>
       </c>
-      <c r="E40" s="34">
+      <c r="E40" s="32">
         <f>E41*$C$41+E45*$C$45+E53*$C$53</f>
         <v>0.56944444444444442</v>
       </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="36" t="s">
+      <c r="A41" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="34">
+      <c r="C41" s="32">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D41" s="34">
+      <c r="D41" s="32">
         <f>AVERAGE(D42:D43)</f>
         <v>0.5</v>
       </c>
-      <c r="E41" s="34">
+      <c r="E41" s="32">
         <f>AVERAGE(E42:E43)</f>
         <v>0.5</v>
       </c>
@@ -2264,10 +2271,10 @@
       <c r="B42" t="s">
         <v>76</v>
       </c>
-      <c r="D42" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E42" s="34">
+      <c r="D42" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E42" s="32">
         <v>0.6</v>
       </c>
     </row>
@@ -2275,26 +2282,26 @@
       <c r="B43" t="s">
         <v>97</v>
       </c>
-      <c r="D43" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E43" s="34">
+      <c r="D43" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E43" s="32">
         <v>0.4</v>
       </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C45" s="34">
+      <c r="C45" s="32">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D45" s="34">
+      <c r="D45" s="32">
         <f>AVERAGE(D46:D51)</f>
         <v>0.35000000000000003</v>
       </c>
-      <c r="E45" s="34">
+      <c r="E45" s="32">
         <f>AVERAGE(E46:E51)</f>
         <v>0.5083333333333333</v>
       </c>
@@ -2303,10 +2310,10 @@
       <c r="B46" t="s">
         <v>80</v>
       </c>
-      <c r="D46" s="34">
+      <c r="D46" s="32">
         <v>0.6</v>
       </c>
-      <c r="E46" s="34">
+      <c r="E46" s="32">
         <v>0.8</v>
       </c>
     </row>
@@ -2314,10 +2321,10 @@
       <c r="B47" t="s">
         <v>77</v>
       </c>
-      <c r="D47" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E47" s="34">
+      <c r="D47" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E47" s="32">
         <v>0.75</v>
       </c>
     </row>
@@ -2325,10 +2332,10 @@
       <c r="B48" t="s">
         <v>78</v>
       </c>
-      <c r="D48" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E48" s="34">
+      <c r="D48" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E48" s="32">
         <v>0.75</v>
       </c>
     </row>
@@ -2336,10 +2343,10 @@
       <c r="B49" t="s">
         <v>79</v>
       </c>
-      <c r="D49" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E49" s="34">
+      <c r="D49" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E49" s="32">
         <v>0.6</v>
       </c>
     </row>
@@ -2347,10 +2354,10 @@
       <c r="B50" t="s">
         <v>95</v>
       </c>
-      <c r="D50" s="34">
+      <c r="D50" s="32">
         <v>0</v>
       </c>
-      <c r="E50" s="34">
+      <c r="E50" s="32">
         <v>0.1</v>
       </c>
     </row>
@@ -2358,26 +2365,26 @@
       <c r="B51" t="s">
         <v>96</v>
       </c>
-      <c r="D51" s="34">
+      <c r="D51" s="32">
         <v>0</v>
       </c>
-      <c r="E51" s="34">
+      <c r="E51" s="32">
         <v>0.05</v>
       </c>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="36" t="s">
+      <c r="A53" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="C53" s="34">
+      <c r="C53" s="32">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D53" s="34">
+      <c r="D53" s="32">
         <f>AVERAGE(D54:D56)</f>
         <v>0.5</v>
       </c>
-      <c r="E53" s="34">
+      <c r="E53" s="32">
         <f>AVERAGE(E54:E56)</f>
         <v>0.70000000000000007</v>
       </c>
@@ -2386,10 +2393,10 @@
       <c r="B54" t="s">
         <v>81</v>
       </c>
-      <c r="D54" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E54" s="34">
+      <c r="D54" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E54" s="32">
         <v>0.75</v>
       </c>
     </row>
@@ -2397,10 +2404,10 @@
       <c r="B55" t="s">
         <v>82</v>
       </c>
-      <c r="D55" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E55" s="34">
+      <c r="D55" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E55" s="32">
         <v>0.6</v>
       </c>
     </row>
@@ -2408,25 +2415,25 @@
       <c r="B56" t="s">
         <v>83</v>
       </c>
-      <c r="D56" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="E56" s="34">
+      <c r="D56" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="E56" s="32">
         <v>0.75</v>
       </c>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="36" t="s">
+      <c r="A58" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="C58" s="34">
-        <v>0.5</v>
-      </c>
-      <c r="D58" s="34">
+      <c r="C58" s="32">
+        <v>0.5</v>
+      </c>
+      <c r="D58" s="32">
         <f>AVERAGE(D59:D60)</f>
         <v>0</v>
       </c>
-      <c r="E58" s="34">
+      <c r="E58" s="32">
         <f>AVERAGE(E59:E60)</f>
         <v>0.05</v>
       </c>
@@ -2435,10 +2442,10 @@
       <c r="B59" t="s">
         <v>85</v>
       </c>
-      <c r="D59" s="34">
+      <c r="D59" s="32">
         <v>0</v>
       </c>
-      <c r="E59" s="34">
+      <c r="E59" s="32">
         <v>0.1</v>
       </c>
     </row>
@@ -2446,10 +2453,10 @@
       <c r="B60" t="s">
         <v>84</v>
       </c>
-      <c r="D60" s="34">
+      <c r="D60" s="32">
         <v>0</v>
       </c>
-      <c r="E60" s="34">
+      <c r="E60" s="32">
         <v>0</v>
       </c>
     </row>
@@ -2488,7 +2495,7 @@
         <f>$B$1*$C$1</f>
         <v>32.5</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="30">
         <v>40576</v>
       </c>
     </row>
@@ -2500,7 +2507,7 @@
         <f t="shared" ref="B3:B14" si="0">$B$1*$C$1</f>
         <v>32.5</v>
       </c>
-      <c r="D3" s="32"/>
+      <c r="D3" s="30"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4">
@@ -2510,7 +2517,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D4" s="32"/>
+      <c r="D4" s="30"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5">
@@ -2520,7 +2527,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="30">
         <v>40597</v>
       </c>
     </row>
@@ -2532,7 +2539,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D6" s="32"/>
+      <c r="D6" s="30"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
@@ -2542,7 +2549,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D7" s="32"/>
+      <c r="D7" s="30"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8">
@@ -2552,7 +2559,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="30"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9">
@@ -2562,7 +2569,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="30"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
@@ -2572,7 +2579,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="30">
         <v>40632</v>
       </c>
     </row>
@@ -2584,7 +2591,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D11" s="32"/>
+      <c r="D11" s="30"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12">
@@ -2594,10 +2601,10 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="30">
         <v>40653</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="30">
         <v>40658</v>
       </c>
     </row>
@@ -2618,7 +2625,7 @@
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="30">
         <v>40667</v>
       </c>
     </row>
@@ -2627,7 +2634,7 @@
         <f>C1*5</f>
         <v>32.5</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="30">
         <v>40693</v>
       </c>
     </row>
@@ -2639,7 +2646,7 @@
         <f>$B$1*$C$15</f>
         <v>162.5</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="30">
         <v>40704</v>
       </c>
     </row>
@@ -2651,7 +2658,7 @@
         <f t="shared" ref="B17:B18" si="1">$B$1*$C$15</f>
         <v>162.5</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="30">
         <v>40711</v>
       </c>
     </row>
@@ -2663,10 +2670,10 @@
         <f t="shared" si="1"/>
         <v>162.5</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="30">
         <v>40715</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="30">
         <v>40718</v>
       </c>
     </row>
@@ -2693,7 +2700,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="33">
+      <c r="A1" s="31">
         <f>B2*D2+B26*D26</f>
         <v>0.5573611111111112</v>
       </c>
@@ -2702,24 +2709,24 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="33">
+      <c r="B2" s="31">
         <f>C3*E3+C16*E16+C22*E22</f>
         <v>0.91472222222222244</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="33"/>
-      <c r="C3" s="34">
+      <c r="B3" s="31"/>
+      <c r="C3" s="32">
         <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
         <v>0.91250000000000009</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="32" t="s">
         <v>53</v>
       </c>
       <c r="E3">
@@ -2728,143 +2735,143 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="D4" s="34">
+      <c r="D4" s="32">
         <f>E5*G5</f>
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="E5" s="34">
+      <c r="E5" s="32">
         <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="D6" s="34">
+      <c r="D6" s="32">
         <f>E7*G7+E8*G8</f>
         <v>0.85000000000000009</v>
       </c>
       <c r="E6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>0.9</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>0.8</v>
       </c>
       <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="D9" s="34">
+      <c r="D9" s="32">
         <f>E10*G10+E11*G11+E12*G12</f>
         <v>0.85</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="E10" s="34">
+      <c r="E10" s="32">
         <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="E11" s="34">
+      <c r="E11" s="32">
         <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="E12" s="34">
+      <c r="E12" s="32">
         <v>0.7</v>
       </c>
       <c r="F12" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="D13" s="34">
+      <c r="D13" s="32">
         <f>E14*G14+E15*G15</f>
         <v>0.95</v>
       </c>
       <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="34">
+      <c r="E14" s="32">
         <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="34">
+      <c r="E15" s="32">
         <v>0.9</v>
       </c>
       <c r="F15" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="C16" s="34">
+      <c r="C16" s="32">
         <f>D17*F17+D18*F18+D21*F21</f>
         <v>0.96500000000000008</v>
       </c>
@@ -2877,58 +2884,58 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="D17" s="34">
+      <c r="D17" s="32">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="34">
+      <c r="F17" s="32">
         <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="D18" s="34">
+      <c r="D18" s="32">
         <f>E19*G19+E20*G20</f>
         <v>1</v>
       </c>
       <c r="E18" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="34">
+      <c r="F18" s="32">
         <v>0.45</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="E19" s="34">
+      <c r="E19" s="32">
         <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="E20" s="34">
+      <c r="E20" s="32">
         <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="D21" s="34">
+      <c r="D21" s="32">
         <v>0.7</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="32">
         <v>0.45</v>
       </c>
     </row>
@@ -2946,7 +2953,7 @@
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="D23" s="34">
+      <c r="D23" s="32">
         <v>1</v>
       </c>
       <c r="E23" t="s">
@@ -2958,7 +2965,7 @@
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="D24" s="34">
+      <c r="D24" s="32">
         <v>1</v>
       </c>
       <c r="E24" t="s">
@@ -2970,7 +2977,7 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="D25" s="34">
+      <c r="D25" s="32">
         <v>0.6</v>
       </c>
       <c r="E25" t="s">
@@ -2982,37 +2989,37 @@
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="34">
+      <c r="B26" s="32">
         <f>C27*E27</f>
         <v>0.2</v>
       </c>
       <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="C27" s="34">
+      <c r="C27" s="32">
         <f>D28*F28</f>
         <v>0.2</v>
       </c>
       <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="D28" s="34">
+      <c r="D28" s="32">
         <v>0.2</v>
       </c>
       <c r="E28" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="34">
+      <c r="F28" s="32">
         <v>1</v>
       </c>
     </row>
@@ -3032,36 +3039,36 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="33">
+      <c r="A1" s="31">
         <f>B2*D2+B26*D26</f>
         <v>0.31430555555555562</v>
       </c>
       <c r="B1" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="32">
+      <c r="D1" s="30">
         <v>40632</v>
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="B2" s="33">
+      <c r="B2" s="31">
         <f>C3*E3+C16*E16+C22*E22</f>
         <v>0.62861111111111123</v>
       </c>
       <c r="C2" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="34">
+      <c r="D2" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="33"/>
-      <c r="C3" s="34">
+      <c r="B3" s="31"/>
+      <c r="C3" s="32">
         <f>D4*F4+D6*F6+D9*F9+D13*F13</f>
         <v>0.72500000000000009</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="32" t="s">
         <v>53</v>
       </c>
       <c r="E3">
@@ -3070,142 +3077,142 @@
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="D4" s="34">
+      <c r="D4" s="32">
         <f>E5*G5</f>
         <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="34">
+      <c r="F4" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
-      <c r="E5" s="34">
+      <c r="E5" s="32">
         <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>49</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="D6" s="34">
+      <c r="D6" s="32">
         <f>E7*G7+E8*G8</f>
         <v>0.85000000000000009</v>
       </c>
       <c r="E6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="34">
+      <c r="F6" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="1:7">
-      <c r="E7" s="34">
+      <c r="E7" s="32">
         <v>0.9</v>
       </c>
       <c r="F7" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="34">
+      <c r="G7" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="8" spans="1:7">
-      <c r="E8" s="34">
+      <c r="E8" s="32">
         <v>0.8</v>
       </c>
       <c r="F8" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="34">
+      <c r="G8" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="D9" s="34">
+      <c r="D9" s="32">
         <f>E10*G10+E11*G11+E12*G12</f>
         <v>0.85</v>
       </c>
       <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="34">
+      <c r="F9" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:7">
-      <c r="E10" s="34">
+      <c r="E10" s="32">
         <v>1</v>
       </c>
       <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="34">
+      <c r="G10" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="E11" s="34">
+      <c r="E11" s="32">
         <v>1</v>
       </c>
       <c r="F11" t="s">
         <v>56</v>
       </c>
-      <c r="G11" s="34">
+      <c r="G11" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="12" spans="1:7">
-      <c r="E12" s="34">
+      <c r="E12" s="32">
         <v>0.7</v>
       </c>
       <c r="F12" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="34">
+      <c r="G12" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:7">
-      <c r="D13" s="34">
+      <c r="D13" s="32">
         <v>0.2</v>
       </c>
       <c r="E13" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="32">
         <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="E14" s="34">
+      <c r="E14" s="32">
         <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="34">
+      <c r="G14" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="E15" s="34">
+      <c r="E15" s="32">
         <v>0.9</v>
       </c>
       <c r="F15" t="s">
         <v>57</v>
       </c>
-      <c r="G15" s="34">
+      <c r="G15" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="C16" s="34">
+      <c r="C16" s="32">
         <f>D17*F17+D18*F18+D21*F21</f>
         <v>0.62750000000000006</v>
       </c>
@@ -3218,57 +3225,57 @@
       </c>
     </row>
     <row r="17" spans="2:7">
-      <c r="D17" s="34">
+      <c r="D17" s="32">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>60</v>
       </c>
-      <c r="F17" s="34">
+      <c r="F17" s="32">
         <v>0.2</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="D18" s="34">
+      <c r="D18" s="32">
         <v>0.75</v>
       </c>
       <c r="E18" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="34">
+      <c r="F18" s="32">
         <v>0.45</v>
       </c>
     </row>
     <row r="19" spans="2:7">
-      <c r="E19" s="34">
+      <c r="E19" s="32">
         <v>1</v>
       </c>
       <c r="F19" t="s">
         <v>62</v>
       </c>
-      <c r="G19" s="34">
+      <c r="G19" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="2:7">
-      <c r="E20" s="34">
+      <c r="E20" s="32">
         <v>1</v>
       </c>
       <c r="F20" t="s">
         <v>63</v>
       </c>
-      <c r="G20" s="34">
+      <c r="G20" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="D21" s="34">
+      <c r="D21" s="32">
         <v>0.2</v>
       </c>
       <c r="E21" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="34">
+      <c r="F21" s="32">
         <v>0.45</v>
       </c>
     </row>
@@ -3286,7 +3293,7 @@
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="D23" s="34">
+      <c r="D23" s="32">
         <v>1</v>
       </c>
       <c r="E23" t="s">
@@ -3298,7 +3305,7 @@
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="D24" s="34">
+      <c r="D24" s="32">
         <v>0.6</v>
       </c>
       <c r="E24" t="s">
@@ -3310,7 +3317,7 @@
       </c>
     </row>
     <row r="25" spans="2:7">
-      <c r="D25" s="34">
+      <c r="D25" s="32">
         <v>0</v>
       </c>
       <c r="E25" t="s">
@@ -3322,37 +3329,37 @@
       </c>
     </row>
     <row r="26" spans="2:7">
-      <c r="B26" s="34">
+      <c r="B26" s="32">
         <f>C27*E27</f>
         <v>0</v>
       </c>
       <c r="C26" t="s">
         <v>68</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="32">
         <v>0.5</v>
       </c>
     </row>
     <row r="27" spans="2:7">
-      <c r="C27" s="34">
+      <c r="C27" s="32">
         <f>D28*F28</f>
         <v>0</v>
       </c>
       <c r="D27" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:7">
-      <c r="D28" s="34">
+      <c r="D28" s="32">
         <v>0</v>
       </c>
       <c r="E28" t="s">
         <v>70</v>
       </c>
-      <c r="F28" s="34">
+      <c r="F28" s="32">
         <v>1</v>
       </c>
     </row>

</xml_diff>